<commit_message>
perbaikan ke sekian kalinya by segap
</commit_message>
<xml_diff>
--- a/public/templates/pegawai_template.xlsx
+++ b/public/templates/pegawai_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SistemDinas-KP\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E82116-9C21-4D97-9CDE-2F6BCC9210B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AC8AC7-FA70-4953-BF81-E396C4C965EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0B7F34EB-B3F1-466B-B3E2-3344792ECD58}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nama</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Golongan</t>
+  </si>
+  <si>
+    <t>Bidang</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F5B234-3A58-41FD-BA52-373721B6FB2E}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,9 +460,10 @@
     <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -484,11 +488,14 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
     </row>
   </sheetData>

</xml_diff>